<commit_message>
session 1 and 2 finished
</commit_message>
<xml_diff>
--- a/Lab2.xlsx
+++ b/Lab2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>loop2</t>
   </si>
@@ -40,13 +40,43 @@
     <t>loop4/loop5</t>
   </si>
   <si>
-    <t>Complexity: O(n^2)</t>
+    <t>O(n^2) FROM LOOP 2</t>
+  </si>
+  <si>
+    <t>O(n^2) FROM LOOP 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Theoretical Complexities</t>
+  </si>
+  <si>
+    <t>O(nlogn) FROM LOOP 1</t>
+  </si>
+  <si>
+    <t>loop 1 has a better complexity than loop 3 because values are smaller than 1</t>
+  </si>
+  <si>
+    <t>loop 3 has a better complexity than loop 2 because values are greater than 1</t>
+  </si>
+  <si>
+    <t>O(n^4) FROM LOOP4</t>
+  </si>
+  <si>
+    <t>O(nlogn) FROM LOOP 5</t>
+  </si>
+  <si>
+    <t>UNKNOWN METHOD:</t>
+  </si>
+  <si>
+    <t>The complexity of this method is O(n^3) as there is 3 nested for loops and are iterative</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -84,9 +114,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -105,7 +143,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -119,7 +157,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -145,7 +182,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -208,7 +245,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -234,7 +270,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -342,6 +378,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-652F-4F3D-8112-C844F7236826}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -409,7 +450,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="234307776"/>
@@ -471,7 +512,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="234301616"/>
@@ -512,7 +553,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -524,7 +565,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -538,7 +579,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -564,7 +604,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -637,7 +677,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -663,7 +702,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -771,6 +810,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8034-4AF1-A5AF-C8C2BC5133E9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -838,7 +882,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="236778976"/>
@@ -900,7 +944,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="236779536"/>
@@ -941,7 +985,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -953,7 +997,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -967,7 +1011,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -993,7 +1036,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1056,7 +1099,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1082,7 +1124,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1190,6 +1232,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-082C-4349-A037-D8F4D81C2B28}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1257,7 +1304,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="168137408"/>
@@ -1319,7 +1366,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="168134608"/>
@@ -1360,7 +1407,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1372,7 +1419,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1386,7 +1433,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1412,13 +1458,23 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.6338454268558892E-2"/>
+          <c:y val="0.19721055701370663"/>
+          <c:w val="0.84216774273078876"/>
+          <c:h val="0.77736111111111106"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -1474,7 +1530,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1500,7 +1555,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1608,6 +1663,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5F8E-4B6F-9C1D-8C1F272604B6}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1675,7 +1735,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="236775056"/>
@@ -1737,7 +1797,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="236772256"/>
@@ -1778,7 +1838,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1790,7 +1850,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1804,7 +1864,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1830,7 +1889,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1893,7 +1952,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1919,7 +1977,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1985,6 +2043,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5A32-4DBA-8E89-70EF84C927E7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2052,7 +2115,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="240943360"/>
@@ -2114,7 +2177,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="240941120"/>
@@ -2155,7 +2218,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2167,7 +2230,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2181,7 +2244,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2207,7 +2269,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2266,11 +2328,10 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="4"/>
+            <c:order val="3"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2296,7 +2357,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-ES"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2362,6 +2423,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C7FF-4378-A866-27F96C4096FE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2429,7 +2495,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="234306656"/>
@@ -2491,7 +2557,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="243371744"/>
@@ -2532,7 +2598,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5883,16 +5949,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2752726</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5913,16 +5979,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>657224</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2781300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5943,16 +6009,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>2843212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5973,16 +6039,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>962024</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>2852737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6003,16 +6069,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6033,16 +6099,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6140,6 +6206,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -6175,6 +6258,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6351,19 +6451,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -6373,8 +6479,14 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8</v>
       </c>
@@ -6390,10 +6502,18 @@
         <f>B2/C2</f>
         <v>1.6956521739130437</v>
       </c>
+      <c r="G2">
+        <f>B2</f>
+        <v>7.8000000000000005E-7</v>
+      </c>
+      <c r="H2">
+        <f>C2</f>
+        <v>4.5999999999999999E-7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>A2*2</f>
+        <f t="shared" ref="A3:A15" si="0">A2*2</f>
         <v>16</v>
       </c>
       <c r="B3">
@@ -6405,13 +6525,21 @@
         <v>1.72E-6</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D15" si="0">B3/C3</f>
+        <f t="shared" ref="D3:D15" si="1">B3/C3</f>
         <v>1.8139534883720931</v>
       </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G15" si="2">A3^2/A2^2 *B2</f>
+        <v>3.1200000000000002E-6</v>
+      </c>
+      <c r="H3">
+        <f>A3^2/A2^2 *C2</f>
+        <v>1.84E-6</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>A3*2</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B4">
@@ -6423,13 +6551,21 @@
         <v>6.1999999999999999E-6</v>
       </c>
       <c r="D4">
+        <f t="shared" si="1"/>
+        <v>2.0161290322580645</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>1.2480000000000001E-5</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H15" si="3">A4^2/A3^2 *C3</f>
+        <v>6.8800000000000002E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
         <f t="shared" si="0"/>
-        <v>2.0161290322580645</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f>A4*2</f>
         <v>64</v>
       </c>
       <c r="B5">
@@ -6441,13 +6577,21 @@
         <v>2.4999999999999998E-5</v>
       </c>
       <c r="D5">
+        <f t="shared" si="1"/>
+        <v>2.52</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>4.9999999999999996E-5</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>2.48E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
         <f t="shared" si="0"/>
-        <v>2.52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f>A5*2</f>
         <v>128</v>
       </c>
       <c r="B6">
@@ -6459,13 +6603,21 @@
         <v>9.3999999999999994E-5</v>
       </c>
       <c r="D6">
+        <f t="shared" si="1"/>
+        <v>1.9893617021276595</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>2.52E-4</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>9.9999999999999991E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
         <f t="shared" si="0"/>
-        <v>1.9893617021276595</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f>A6*2</f>
         <v>256</v>
       </c>
       <c r="B7">
@@ -6477,13 +6629,21 @@
         <v>3.8999999999999999E-4</v>
       </c>
       <c r="D7">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000004</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>7.4799999999999997E-4</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>3.7599999999999998E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
         <f t="shared" si="0"/>
-        <v>2.0000000000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f>A7*2</f>
         <v>512</v>
       </c>
       <c r="B8">
@@ -6495,13 +6655,21 @@
         <v>1.5600000000000002E-3</v>
       </c>
       <c r="D8">
+        <f t="shared" si="1"/>
+        <v>1.903846153846154</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>3.1200000000000004E-3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>1.56E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
         <f t="shared" si="0"/>
-        <v>1.903846153846154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f>A8*2</f>
         <v>1024</v>
       </c>
       <c r="B9">
@@ -6513,13 +6681,21 @@
         <v>6.2000000000000006E-3</v>
       </c>
       <c r="D9">
+        <f t="shared" si="1"/>
+        <v>2.0161290322580645</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>1.1880000000000002E-2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>6.2400000000000008E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
         <f t="shared" si="0"/>
-        <v>2.0161290322580645</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f>A9*2</f>
         <v>2048</v>
       </c>
       <c r="B10">
@@ -6531,13 +6707,21 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="D10">
+        <f t="shared" si="1"/>
+        <v>1.92</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>2.4800000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
         <f t="shared" si="0"/>
-        <v>1.92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f>A10*2</f>
         <v>4096</v>
       </c>
       <c r="B11">
@@ -6549,13 +6733,21 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2.1827956989247315</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>0.192</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
         <f t="shared" si="0"/>
-        <v>2.1827956989247315</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f>A11*2</f>
         <v>8192</v>
       </c>
       <c r="B12">
@@ -6567,13 +6759,21 @@
         <v>0.40600000000000003</v>
       </c>
       <c r="D12">
+        <f t="shared" si="1"/>
+        <v>1.9975369458128078</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>0.372</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
         <f t="shared" si="0"/>
-        <v>1.9975369458128078</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f>A12*2</f>
         <v>16384</v>
       </c>
       <c r="B13">
@@ -6585,13 +6785,21 @@
         <v>1.6220000000000001</v>
       </c>
       <c r="D13">
+        <f t="shared" si="1"/>
+        <v>1.9722564734895192</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>3.2440000000000002</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>1.6240000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
         <f t="shared" si="0"/>
-        <v>1.9722564734895192</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f>A13*2</f>
         <v>32768</v>
       </c>
       <c r="B14">
@@ -6603,13 +6811,21 @@
         <v>6.383</v>
       </c>
       <c r="D14">
+        <f t="shared" si="1"/>
+        <v>1.9943600187999373</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>12.796000000000001</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>6.4880000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
         <f t="shared" si="0"/>
-        <v>1.9943600187999373</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f>A14*2</f>
         <v>65536</v>
       </c>
       <c r="B15">
@@ -6621,17 +6837,33 @@
         <v>25.523</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9974924577831759</v>
       </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>50.92</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>25.532</v>
+      </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>8</v>
-      </c>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="G16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" ht="226.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="1"/>
+      <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -6643,6 +6875,12 @@
       <c r="D18" t="s">
         <v>4</v>
       </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -6660,10 +6898,18 @@
         <f>C19/B19</f>
         <v>0.60256410256410253</v>
       </c>
+      <c r="G19">
+        <f>B19</f>
+        <v>7.8000000000000005E-7</v>
+      </c>
+      <c r="H19" s="3">
+        <f>C19</f>
+        <v>4.7E-7</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>A19*2</f>
+        <f t="shared" ref="A20:A32" si="4">A19*2</f>
         <v>16</v>
       </c>
       <c r="B20">
@@ -6675,13 +6921,21 @@
         <v>9.2999999999999999E-7</v>
       </c>
       <c r="D20">
-        <f t="shared" ref="D20:D32" si="1">C20/B20</f>
+        <f t="shared" ref="D20:D32" si="5">C20/B20</f>
         <v>0.29807692307692307</v>
+      </c>
+      <c r="G20">
+        <f>A20^2/A19^2*B19</f>
+        <v>3.1200000000000002E-6</v>
+      </c>
+      <c r="H20" s="3">
+        <f>A20/A19*LOG10(A20)/LOG10(A19)*C19</f>
+        <v>1.2533333333333335E-6</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>A20*2</f>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="B21">
@@ -6693,13 +6947,21 @@
         <v>2.34E-6</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.18720000000000003</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G21:G32" si="6">A21^2/A20^2 *B20</f>
+        <v>1.2480000000000001E-5</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" ref="H21:H32" si="7">A21/A20*LOG10(A21)/LOG10(A20)*C20</f>
+        <v>2.3249999999999998E-6</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>A21*2</f>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="B22">
@@ -6711,13 +6973,21 @@
         <v>5.31E-6</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>8.4285714285714283E-2</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="6"/>
+        <v>4.9999999999999996E-5</v>
+      </c>
+      <c r="H22" s="3">
+        <f t="shared" si="7"/>
+        <v>5.6160000000000001E-6</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>A22*2</f>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="B23">
@@ -6729,13 +6999,21 @@
         <v>1.2330000000000001E-5</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6.5935828877005359E-2</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="6"/>
+        <v>2.52E-4</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" si="7"/>
+        <v>1.239E-5</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>A23*2</f>
+        <f t="shared" si="4"/>
         <v>256</v>
       </c>
       <c r="B24">
@@ -6747,13 +7025,21 @@
         <v>2.7310000000000001E-5</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3.5012820512820508E-2</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="6"/>
+        <v>7.4799999999999997E-4</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="7"/>
+        <v>2.8182857142857141E-5</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>A24*2</f>
+        <f t="shared" si="4"/>
         <v>512</v>
       </c>
       <c r="B25">
@@ -6765,13 +7051,21 @@
         <v>6.2000000000000003E-5</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2.0875420875420873E-2</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="6"/>
+        <v>3.1200000000000004E-3</v>
+      </c>
+      <c r="H25" s="3">
+        <f>A25/A24*LOG10(A25)/LOG10(A24)*C24</f>
+        <v>6.1447500000000004E-5</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>A25*2</f>
+        <f t="shared" si="4"/>
         <v>1024</v>
       </c>
       <c r="B26">
@@ -6783,13 +7077,21 @@
         <v>1.25E-4</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0.01</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="6"/>
+        <v>1.1880000000000002E-2</v>
+      </c>
+      <c r="H26" s="3">
+        <f t="shared" si="7"/>
+        <v>1.3777777777777779E-4</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>A26*2</f>
+        <f t="shared" si="4"/>
         <v>2048</v>
       </c>
       <c r="B27">
@@ -6801,13 +7103,21 @@
         <v>2.9599999999999998E-4</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6.1666666666666667E-3</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="6"/>
+        <v>0.05</v>
+      </c>
+      <c r="H27" s="3">
+        <f t="shared" si="7"/>
+        <v>2.7500000000000002E-4</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>A27*2</f>
+        <f t="shared" si="4"/>
         <v>4096</v>
       </c>
       <c r="B28">
@@ -6819,13 +7129,21 @@
         <v>6.2399999999999999E-4</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3.0738916256157632E-3</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="6"/>
+        <v>0.192</v>
+      </c>
+      <c r="H28" s="3">
+        <f t="shared" si="7"/>
+        <v>6.4581818181818176E-4</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>A28*2</f>
+        <f t="shared" si="4"/>
         <v>8192</v>
       </c>
       <c r="B29">
@@ -6837,13 +7155,21 @@
         <v>1.374E-3</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.694204685573366E-3</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="6"/>
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="H29" s="3">
+        <f t="shared" si="7"/>
+        <v>1.3519999999999999E-3</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>A29*2</f>
+        <f t="shared" si="4"/>
         <v>16384</v>
       </c>
       <c r="B30">
@@ -6855,13 +7181,21 @@
         <v>2.9029999999999998E-3</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9.07471084713973E-4</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="6"/>
+        <v>3.2440000000000002</v>
+      </c>
+      <c r="H30" s="3">
+        <f t="shared" si="7"/>
+        <v>2.9593846153846155E-3</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>A30*2</f>
+        <f t="shared" si="4"/>
         <v>32768</v>
       </c>
       <c r="B31">
@@ -6873,13 +7207,21 @@
         <v>6.241E-3</v>
       </c>
       <c r="D31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>4.9025923016496461E-4</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="6"/>
+        <v>12.796000000000001</v>
+      </c>
+      <c r="H31" s="3">
+        <f t="shared" si="7"/>
+        <v>6.2207142857142851E-3</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>A31*2</f>
+        <f t="shared" si="4"/>
         <v>65536</v>
       </c>
       <c r="B32">
@@ -6891,16 +7233,35 @@
         <v>1.3290999999999999E-2</v>
       </c>
       <c r="D32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>2.6069985485073163E-4</v>
       </c>
+      <c r="G32">
+        <f t="shared" si="6"/>
+        <v>50.92</v>
+      </c>
+      <c r="H32" s="3">
+        <f t="shared" si="7"/>
+        <v>1.3314133333333334E-2</v>
+      </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G34" s="1" t="s">
-        <v>8</v>
-      </c>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="G33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="4"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="239.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>5</v>
       </c>
@@ -6910,8 +7271,14 @@
       <c r="D35" t="s">
         <v>7</v>
       </c>
+      <c r="G35" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>8</v>
       </c>
@@ -6927,10 +7294,18 @@
         <f>B36/C36</f>
         <v>2.2660098522167491</v>
       </c>
+      <c r="G36">
+        <f>B36</f>
+        <v>4.6E-5</v>
+      </c>
+      <c r="H36">
+        <f>C36</f>
+        <v>2.0299999999999999E-5</v>
+      </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>A36*2</f>
+        <f t="shared" ref="A37:A42" si="8">A36*2</f>
         <v>16</v>
       </c>
       <c r="B37">
@@ -6942,13 +7317,21 @@
         <v>2.03E-4</v>
       </c>
       <c r="D37">
-        <f t="shared" ref="D37:D42" si="2">B37/C37</f>
+        <f t="shared" ref="D37:D42" si="9">B37/C37</f>
         <v>4.458128078817734</v>
       </c>
+      <c r="G37">
+        <f>$A37^4/$A36^4 *B36</f>
+        <v>7.36E-4</v>
+      </c>
+      <c r="H37">
+        <f>$A37^3/$A36^3 *LOG10(A37)/LOG10(A36)*C36</f>
+        <v>2.1653333333333336E-4</v>
+      </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f>A37*2</f>
+        <f t="shared" si="8"/>
         <v>32</v>
       </c>
       <c r="B38">
@@ -6960,13 +7343,21 @@
         <v>2.0200000000000001E-3</v>
       </c>
       <c r="D38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>6.1881188118811883</v>
       </c>
+      <c r="G38">
+        <f t="shared" ref="G38:G42" si="10">$A38^4/$A37^4 *B37</f>
+        <v>1.448E-2</v>
+      </c>
+      <c r="H38">
+        <f t="shared" ref="H38:H42" si="11">$A38^3/$A37^3 *LOG10(A38)/LOG10(A37)*C37</f>
+        <v>2.0300000000000001E-3</v>
+      </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f>A38*2</f>
+        <f t="shared" si="8"/>
         <v>64</v>
       </c>
       <c r="B39">
@@ -6978,13 +7369,21 @@
         <v>1.8700000000000001E-2</v>
       </c>
       <c r="D39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>10.855614973262032</v>
       </c>
+      <c r="G39">
+        <f t="shared" si="10"/>
+        <v>0.2</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="11"/>
+        <v>1.9392E-2</v>
+      </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f>A39*2</f>
+        <f t="shared" si="8"/>
         <v>128</v>
       </c>
       <c r="B40">
@@ -6996,13 +7395,21 @@
         <v>0.17100000000000001</v>
       </c>
       <c r="D40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>18.701754385964911</v>
       </c>
+      <c r="G40">
+        <f t="shared" si="10"/>
+        <v>3.2480000000000002</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="11"/>
+        <v>0.17453333333333335</v>
+      </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f>A40*2</f>
+        <f t="shared" si="8"/>
         <v>256</v>
       </c>
       <c r="B41">
@@ -7014,13 +7421,21 @@
         <v>1.6380000000000001</v>
       </c>
       <c r="D41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>31.112942612942611</v>
       </c>
+      <c r="G41">
+        <f t="shared" si="10"/>
+        <v>51.167999999999999</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="11"/>
+        <v>1.5634285714285714</v>
+      </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>A41*2</f>
+        <f t="shared" si="8"/>
         <v>512</v>
       </c>
       <c r="B42">
@@ -7032,11 +7447,48 @@
         <v>14.557</v>
       </c>
       <c r="D42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="9"/>
         <v>56.068764168441298</v>
       </c>
+      <c r="G42">
+        <f t="shared" si="10"/>
+        <v>815.40800000000002</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="11"/>
+        <v>14.742000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="5"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="A58:F58"/>
+    <mergeCell ref="A57:B57"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>